<commit_message>
Security Test Results Rubric Completed
</commit_message>
<xml_diff>
--- a/Testing/SecurityTestingResults.xlsx
+++ b/Testing/SecurityTestingResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4f1fdb1c965c762b/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB5832F5-5721-423D-B470-063290881A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{BB5832F5-5721-423D-B470-063290881A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0341C6E-2743-4E27-BCE1-35ADD8910950}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{CAD017A8-3FF2-41FC-A736-6968CD04B18D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Testing Action</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Test 2</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Security Testing Results Sheet</t>
   </si>
   <si>
@@ -75,6 +72,15 @@
   </si>
   <si>
     <t xml:space="preserve"> Needs to show error message.</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes attached on Code and Security Testing Results (written) markdown </t>
   </si>
 </sst>
 </file>
@@ -488,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A5B3C56-111D-47BF-99CF-C807DC20AF37}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,12 +509,12 @@
     <col min="5" max="5" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -525,38 +531,41 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>